<commit_message>
Bunch of functions to parse excell formulas
</commit_message>
<xml_diff>
--- a/Submarine/PodmornicaLast.xlsx
+++ b/Submarine/PodmornicaLast.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\DRIVE2\Projects\STEM GAMES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\STEM\git\Submarine\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098B4D5F-582F-4819-8775-A96947798CA8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7610"/>
+    <workbookView xWindow="3945" yWindow="1155" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Podmornica" sheetId="1" r:id="rId1"/>
@@ -65,10 +66,16 @@
     <definedName name="solver_val" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -725,7 +732,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -1024,7 +1031,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1038,7 +1045,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1182,6 +1188,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-89A4-4C0D-844A-8A2A2A68F6F8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1364,7 +1375,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1378,7 +1389,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1498,6 +1508,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E938-4880-91E1-F6486895EFC3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1583,6 +1598,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E938-4880-91E1-F6486895EFC3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1668,6 +1688,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E938-4880-91E1-F6486895EFC3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1753,6 +1778,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E938-4880-91E1-F6486895EFC3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -1838,6 +1868,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-E938-4880-91E1-F6486895EFC3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1984,7 +2019,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2052,7 +2086,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2066,7 +2100,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2189,6 +2222,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AD74-4C26-923D-42A671CC377D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2277,6 +2315,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AD74-4C26-923D-42A671CC377D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2365,6 +2408,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AD74-4C26-923D-42A671CC377D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -2453,6 +2501,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-AD74-4C26-923D-42A671CC377D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -2541,6 +2594,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-AD74-4C26-923D-42A671CC377D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2687,7 +2745,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2755,7 +2812,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2769,7 +2826,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2863,6 +2919,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B2D1-44C9-A254-3524C1E25D12}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -5285,7 +5346,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Arrow Connector 2"/>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -5332,7 +5399,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="6" name="Straight Arrow Connector 5"/>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -5379,7 +5452,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5409,7 +5488,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5439,7 +5524,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5469,7 +5560,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5749,38 +5846,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:AQ206"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="H109" colorId="8" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="M111" sqref="M111"/>
+    <sheetView tabSelected="1" defaultGridColor="0" colorId="8" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="48"/>
-    <col min="2" max="2" width="35.90625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="22.81640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.90625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30.54296875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="27.1796875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.54296875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.08984375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="23.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="43.54296875" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="13.90625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.453125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12.90625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="48"/>
+    <col min="2" max="2" width="35.85546875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="22.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="43.5703125" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" style="1" customWidth="1"/>
     <col min="15" max="15" width="13" style="1" customWidth="1"/>
-    <col min="16" max="17" width="8.90625" style="1"/>
-    <col min="18" max="23" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="8.90625" style="1"/>
+    <col min="16" max="17" width="8.85546875" style="1"/>
+    <col min="18" max="23" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="48">
         <v>1</v>
       </c>
@@ -5788,7 +5885,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>203</v>
       </c>
@@ -5799,7 +5896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>204</v>
       </c>
@@ -5810,7 +5907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -5821,7 +5918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="48">
         <v>2</v>
       </c>
@@ -5829,7 +5926,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -5840,7 +5937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>210</v>
       </c>
@@ -5848,7 +5945,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>123</v>
       </c>
@@ -5859,7 +5956,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>124</v>
       </c>
@@ -5870,7 +5967,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>191</v>
       </c>
@@ -5881,7 +5978,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>209</v>
       </c>
@@ -5892,7 +5989,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="48">
         <v>3</v>
       </c>
@@ -5900,7 +5997,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
@@ -5912,7 +6009,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>17</v>
       </c>
@@ -5924,7 +6021,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
@@ -5935,7 +6032,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="48">
         <v>4</v>
       </c>
@@ -5946,7 +6043,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>40</v>
       </c>
@@ -5958,7 +6055,7 @@
         <v>11.047767954145339</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>10</v>
       </c>
@@ -5970,7 +6067,7 @@
       </c>
       <c r="I22" s="5"/>
     </row>
-    <row r="23" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>174</v>
       </c>
@@ -5979,7 +6076,7 @@
       </c>
       <c r="I23" s="5"/>
     </row>
-    <row r="24" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>185</v>
       </c>
@@ -5989,7 +6086,7 @@
       </c>
       <c r="I24" s="5"/>
     </row>
-    <row r="25" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>59</v>
       </c>
@@ -5999,7 +6096,7 @@
       </c>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>78</v>
       </c>
@@ -6009,10 +6106,10 @@
       </c>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="48">
         <v>5</v>
       </c>
@@ -6021,7 +6118,7 @@
       </c>
       <c r="I28" s="5"/>
     </row>
-    <row r="29" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>170</v>
       </c>
@@ -6034,7 +6131,7 @@
       </c>
       <c r="I29" s="5"/>
     </row>
-    <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>15</v>
       </c>
@@ -6047,7 +6144,7 @@
       </c>
       <c r="I30" s="5"/>
     </row>
-    <row r="31" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>24</v>
       </c>
@@ -6060,10 +6157,10 @@
       </c>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I32" s="5"/>
     </row>
-    <row r="33" spans="1:43" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A33" s="48">
         <v>6</v>
       </c>
@@ -6072,7 +6169,7 @@
       </c>
       <c r="I33" s="5"/>
     </row>
-    <row r="34" spans="1:43" ht="18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
         <v>169</v>
       </c>
@@ -6085,7 +6182,7 @@
       </c>
       <c r="I34" s="5"/>
     </row>
-    <row r="35" spans="1:43" ht="18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
         <v>105</v>
       </c>
@@ -6098,7 +6195,7 @@
       </c>
       <c r="I35" s="5"/>
     </row>
-    <row r="36" spans="1:43" ht="18" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
         <v>38</v>
       </c>
@@ -6111,7 +6208,7 @@
       </c>
       <c r="I36" s="5"/>
     </row>
-    <row r="37" spans="1:43" ht="18" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>37</v>
       </c>
@@ -6142,7 +6239,7 @@
       <c r="AP37" s="2"/>
       <c r="AQ37" s="2"/>
     </row>
-    <row r="38" spans="1:43" ht="18" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
         <v>16</v>
       </c>
@@ -6169,7 +6266,7 @@
       <c r="AP38" s="2"/>
       <c r="AQ38" s="2"/>
     </row>
-    <row r="39" spans="1:43" ht="18" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
         <v>34</v>
       </c>
@@ -6207,7 +6304,7 @@
       <c r="AP39" s="2"/>
       <c r="AQ39" s="2"/>
     </row>
-    <row r="40" spans="1:43" ht="18" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
         <v>17</v>
       </c>
@@ -6238,7 +6335,7 @@
       <c r="AP40" s="2"/>
       <c r="AQ40" s="2"/>
     </row>
-    <row r="41" spans="1:43" ht="18" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
         <v>60</v>
       </c>
@@ -6269,7 +6366,7 @@
       <c r="AP41" s="2"/>
       <c r="AQ41" s="2"/>
     </row>
-    <row r="42" spans="1:43" ht="18" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
         <v>18</v>
       </c>
@@ -6299,7 +6396,7 @@
       <c r="AP42" s="2"/>
       <c r="AQ42" s="2"/>
     </row>
-    <row r="43" spans="1:43" ht="18" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
         <v>20</v>
       </c>
@@ -6326,7 +6423,7 @@
       <c r="AP43" s="2"/>
       <c r="AQ43" s="2"/>
     </row>
-    <row r="44" spans="1:43" ht="18" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:43" x14ac:dyDescent="0.3">
       <c r="R44" s="2"/>
       <c r="S44" s="2"/>
       <c r="T44" s="2"/>
@@ -6346,7 +6443,7 @@
       <c r="AP44" s="2"/>
       <c r="AQ44" s="2"/>
     </row>
-    <row r="45" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A45" s="48">
         <v>7</v>
       </c>
@@ -6372,7 +6469,7 @@
       <c r="AP45" s="2"/>
       <c r="AQ45" s="2"/>
     </row>
-    <row r="46" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B46" s="6" t="s">
         <v>62</v>
       </c>
@@ -6384,7 +6481,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="48">
         <v>8</v>
       </c>
@@ -6392,7 +6489,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B50" s="1" t="s">
         <v>26</v>
       </c>
@@ -6411,7 +6508,7 @@
         <v>0.51444444444444448</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B51" s="1" t="s">
         <v>26</v>
       </c>
@@ -6423,7 +6520,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B52" s="1" t="s">
         <v>80</v>
       </c>
@@ -6432,7 +6529,7 @@
         <v>0.31871056437307255</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B53" s="1" t="s">
         <v>23</v>
       </c>
@@ -6441,7 +6538,7 @@
         <v>2.3664460170731748E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B54" s="1" t="s">
         <v>30</v>
       </c>
@@ -6452,7 +6549,7 @@
       <c r="G54" s="8"/>
       <c r="H54" s="5"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B55" s="1" t="s">
         <v>82</v>
       </c>
@@ -6465,7 +6562,7 @@
       <c r="G55" s="8"/>
       <c r="H55" s="5"/>
     </row>
-    <row r="56" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B56" s="1" t="s">
         <v>77</v>
       </c>
@@ -6476,7 +6573,7 @@
       <c r="G56" s="8"/>
       <c r="H56" s="5"/>
     </row>
-    <row r="57" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B57" s="10" t="s">
         <v>85</v>
       </c>
@@ -6484,7 +6581,7 @@
       <c r="G57" s="8"/>
       <c r="H57" s="5"/>
     </row>
-    <row r="58" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B58" s="10" t="s">
         <v>79</v>
       </c>
@@ -6494,7 +6591,7 @@
       </c>
       <c r="H58" s="5"/>
     </row>
-    <row r="59" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B59" s="1" t="s">
         <v>81</v>
       </c>
@@ -6507,7 +6604,7 @@
       </c>
       <c r="H59" s="3"/>
     </row>
-    <row r="60" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B60" s="1" t="s">
         <v>25</v>
       </c>
@@ -6520,7 +6617,7 @@
       </c>
       <c r="H60" s="3"/>
     </row>
-    <row r="61" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B61" s="1" t="s">
         <v>83</v>
       </c>
@@ -6532,7 +6629,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B62" s="12" t="s">
         <v>99</v>
       </c>
@@ -6546,7 +6643,7 @@
       <c r="N62" s="12"/>
       <c r="O62" s="12"/>
     </row>
-    <row r="63" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B63" s="1" t="s">
         <v>84</v>
       </c>
@@ -6554,7 +6651,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B64" s="1" t="s">
         <v>104</v>
       </c>
@@ -6566,10 +6663,10 @@
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:32" x14ac:dyDescent="0.3">
       <c r="E65" s="2"/>
     </row>
-    <row r="66" spans="1:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:32" x14ac:dyDescent="0.3">
       <c r="E66" s="1" t="s">
         <v>192</v>
       </c>
@@ -6577,7 +6674,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="67" spans="1:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A67" s="48">
         <v>9</v>
       </c>
@@ -6586,7 +6683,7 @@
       </c>
       <c r="E67" s="2"/>
     </row>
-    <row r="68" spans="1:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B68" s="1" t="s">
         <v>186</v>
       </c>
@@ -6601,7 +6698,7 @@
         <v>1.2651025112282941</v>
       </c>
     </row>
-    <row r="69" spans="1:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B69" s="1" t="s">
         <v>188</v>
       </c>
@@ -6616,7 +6713,7 @@
         <v>1.1069646973247573</v>
       </c>
     </row>
-    <row r="71" spans="1:32" ht="18.649999999999999" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:32" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="48">
         <v>10</v>
       </c>
@@ -6624,7 +6721,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="72" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B72" s="26"/>
       <c r="C72" s="27"/>
       <c r="D72" s="27" t="s">
@@ -6653,7 +6750,7 @@
       </c>
       <c r="P72" s="30"/>
     </row>
-    <row r="73" spans="1:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B73" s="31"/>
       <c r="C73" s="32"/>
       <c r="D73" s="32"/>
@@ -6682,7 +6779,7 @@
       <c r="AE73" s="2"/>
       <c r="AF73" s="2"/>
     </row>
-    <row r="74" spans="1:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B74" s="31" t="s">
         <v>172</v>
       </c>
@@ -6732,7 +6829,7 @@
       <c r="AE74" s="2"/>
       <c r="AF74" s="2"/>
     </row>
-    <row r="75" spans="1:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B75" s="31" t="s">
         <v>171</v>
       </c>
@@ -6778,7 +6875,7 @@
       <c r="AE75" s="2"/>
       <c r="AF75" s="2"/>
     </row>
-    <row r="76" spans="1:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B76" s="31" t="s">
         <v>180</v>
       </c>
@@ -6823,7 +6920,7 @@
       <c r="AE76" s="2"/>
       <c r="AF76" s="2"/>
     </row>
-    <row r="77" spans="1:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B77" s="31" t="s">
         <v>181</v>
       </c>
@@ -6869,7 +6966,7 @@
       <c r="AE77" s="2"/>
       <c r="AF77" s="2"/>
     </row>
-    <row r="78" spans="1:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B78" s="31" t="s">
         <v>182</v>
       </c>
@@ -6915,7 +7012,7 @@
       <c r="AE78" s="2"/>
       <c r="AF78" s="2"/>
     </row>
-    <row r="79" spans="1:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B79" s="31" t="s">
         <v>196</v>
       </c>
@@ -6962,7 +7059,7 @@
       <c r="AE79" s="2"/>
       <c r="AF79" s="2"/>
     </row>
-    <row r="80" spans="1:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B80" s="31" t="s">
         <v>184</v>
       </c>
@@ -7008,7 +7105,7 @@
       <c r="AE80" s="2"/>
       <c r="AF80" s="2"/>
     </row>
-    <row r="81" spans="2:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B81" s="31" t="s">
         <v>183</v>
       </c>
@@ -7054,7 +7151,7 @@
       <c r="AE81" s="2"/>
       <c r="AF81" s="2"/>
     </row>
-    <row r="82" spans="2:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B82" s="31" t="s">
         <v>194</v>
       </c>
@@ -7094,7 +7191,7 @@
       <c r="AE82" s="2"/>
       <c r="AF82" s="2"/>
     </row>
-    <row r="83" spans="2:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B83" s="31"/>
       <c r="C83" s="32"/>
       <c r="D83" s="32"/>
@@ -7123,7 +7220,7 @@
       <c r="AE83" s="2"/>
       <c r="AF83" s="2"/>
     </row>
-    <row r="84" spans="2:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B84" s="31" t="s">
         <v>179</v>
       </c>
@@ -7171,7 +7268,7 @@
       <c r="AE84" s="2"/>
       <c r="AF84" s="2"/>
     </row>
-    <row r="85" spans="2:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B85" s="31" t="s">
         <v>178</v>
       </c>
@@ -7219,7 +7316,7 @@
       <c r="AE85" s="2"/>
       <c r="AF85" s="2"/>
     </row>
-    <row r="86" spans="2:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B86" s="31" t="s">
         <v>177</v>
       </c>
@@ -7267,7 +7364,7 @@
       <c r="AE86" s="2"/>
       <c r="AF86" s="2"/>
     </row>
-    <row r="87" spans="2:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B87" s="31" t="s">
         <v>48</v>
       </c>
@@ -7317,7 +7414,7 @@
       <c r="AE87" s="2"/>
       <c r="AF87" s="2"/>
     </row>
-    <row r="88" spans="2:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B88" s="31" t="s">
         <v>47</v>
       </c>
@@ -7367,7 +7464,7 @@
       <c r="AE88" s="2"/>
       <c r="AF88" s="2"/>
     </row>
-    <row r="89" spans="2:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B89" s="31"/>
       <c r="C89" s="32"/>
       <c r="D89" s="32"/>
@@ -7384,7 +7481,7 @@
       <c r="O89" s="32"/>
       <c r="P89" s="35"/>
     </row>
-    <row r="90" spans="2:32" x14ac:dyDescent="0.45">
+    <row r="90" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B90" s="31"/>
       <c r="C90" s="32"/>
       <c r="D90" s="33"/>
@@ -7417,7 +7514,7 @@
       <c r="AE90" s="2"/>
       <c r="AF90" s="2"/>
     </row>
-    <row r="91" spans="2:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B91" s="31"/>
       <c r="C91" s="32"/>
       <c r="D91" s="32"/>
@@ -7446,7 +7543,7 @@
       <c r="AE91" s="2"/>
       <c r="AF91" s="2"/>
     </row>
-    <row r="92" spans="2:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B92" s="31"/>
       <c r="C92" s="32"/>
       <c r="D92" s="32"/>
@@ -7492,7 +7589,7 @@
       <c r="AE92" s="2"/>
       <c r="AF92" s="2"/>
     </row>
-    <row r="93" spans="2:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B93" s="31"/>
       <c r="C93" s="32"/>
       <c r="D93" s="32"/>
@@ -7526,7 +7623,7 @@
       <c r="AE93" s="2"/>
       <c r="AF93" s="2"/>
     </row>
-    <row r="94" spans="2:32" x14ac:dyDescent="0.45">
+    <row r="94" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B94" s="31"/>
       <c r="C94" s="32"/>
       <c r="D94" s="32"/>
@@ -7548,7 +7645,7 @@
       <c r="O94" s="32"/>
       <c r="P94" s="35"/>
     </row>
-    <row r="95" spans="2:32" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="95" spans="2:32" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B95" s="42"/>
       <c r="C95" s="43"/>
       <c r="D95" s="43"/>
@@ -7570,10 +7667,10 @@
       <c r="O95" s="43"/>
       <c r="P95" s="45"/>
     </row>
-    <row r="96" spans="2:32" ht="18" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:32" x14ac:dyDescent="0.3">
       <c r="D96" s="11"/>
     </row>
-    <row r="97" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H97" s="3"/>
       <c r="M97" s="1" t="s">
         <v>197</v>
@@ -7582,7 +7679,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
       <c r="E98" s="1" t="s">
         <v>92</v>
       </c>
@@ -7602,7 +7699,7 @@
         <v>7.0200456960690003</v>
       </c>
     </row>
-    <row r="99" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L99" s="1" t="s">
         <v>199</v>
       </c>
@@ -7615,7 +7712,7 @@
         <v>1.9161682770939992</v>
       </c>
     </row>
-    <row r="100" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L100" s="3"/>
       <c r="M100" s="1" t="s">
         <v>200</v>
@@ -7625,7 +7722,7 @@
         <v>0.283831722906001</v>
       </c>
     </row>
-    <row r="101" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M101" s="1" t="s">
         <v>201</v>
       </c>
@@ -7634,7 +7731,7 @@
         <v>-4.9543039310000481E-3</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A102" s="48">
         <v>11</v>
       </c>
@@ -7642,7 +7739,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="103" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L103" s="1" t="s">
         <v>213</v>
       </c>
@@ -7654,7 +7751,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="104" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B104" s="1" t="s">
         <v>39</v>
       </c>
@@ -7672,7 +7769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B106" s="6" t="s">
         <v>53</v>
       </c>
@@ -7684,7 +7781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B107" s="1" t="s">
         <v>43</v>
       </c>
@@ -7696,7 +7793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B108" s="1" t="s">
         <v>44</v>
       </c>
@@ -7708,7 +7805,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="109" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B109" s="1" t="s">
         <v>45</v>
       </c>
@@ -7720,7 +7817,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="110" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B110" s="1" t="s">
         <v>58</v>
       </c>
@@ -7732,7 +7829,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="111" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B111" s="1" t="s">
         <v>41</v>
       </c>
@@ -7744,7 +7841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B112" s="1" t="s">
         <v>42</v>
       </c>
@@ -7756,7 +7853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B113" s="1" t="s">
         <v>93</v>
       </c>
@@ -7768,12 +7865,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
       <c r="J114" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="115" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L115" s="22">
         <v>5</v>
       </c>
@@ -7787,7 +7884,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="116" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A116" s="48">
         <v>12</v>
       </c>
@@ -7814,7 +7911,7 @@
         <v>28.682944670571846</v>
       </c>
     </row>
-    <row r="117" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I117" s="1" t="s">
         <v>178</v>
       </c>
@@ -7835,7 +7932,7 @@
         <v>94.794422369265192</v>
       </c>
     </row>
-    <row r="118" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B118" s="12" t="s">
         <v>52</v>
       </c>
@@ -7862,7 +7959,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="119" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B119" s="1" t="s">
         <v>165</v>
       </c>
@@ -7905,7 +8002,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="120" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B120" s="1" t="s">
         <v>166</v>
       </c>
@@ -7941,7 +8038,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="121" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B121" s="1" t="s">
         <v>167</v>
       </c>
@@ -7959,7 +8056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B122" s="1" t="s">
         <v>157</v>
       </c>
@@ -7992,7 +8089,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="123" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B123" s="1" t="s">
         <v>168</v>
       </c>
@@ -8028,7 +8125,7 @@
         <v>67.34340040956603</v>
       </c>
     </row>
-    <row r="124" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D124" s="2"/>
       <c r="E124" s="2">
         <f>SUM(E119:E123)</f>
@@ -8054,7 +8151,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="125" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
       <c r="I125" s="1" t="s">
@@ -8077,7 +8174,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="126" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D126" s="2"/>
       <c r="E126" s="2"/>
       <c r="I126" s="1" t="s">
@@ -8100,7 +8197,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="127" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
       <c r="E127" s="2"/>
       <c r="I127" s="1" t="s">
         <v>47</v>
@@ -8122,7 +8219,7 @@
         <v>82.331499535408255</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="48">
         <v>13</v>
       </c>
@@ -8131,7 +8228,7 @@
       </c>
       <c r="E129" s="2"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B130" s="1" t="s">
         <v>114</v>
       </c>
@@ -8143,7 +8240,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E131" s="2"/>
       <c r="H131" s="1">
         <v>20</v>
@@ -8152,7 +8249,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B132" s="1" t="s">
         <v>121</v>
       </c>
@@ -8170,7 +8267,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B133" s="1" t="s">
         <v>123</v>
       </c>
@@ -8197,7 +8294,7 @@
         <v>1435</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B134" s="1" t="s">
         <v>124</v>
       </c>
@@ -8224,7 +8321,7 @@
         <v>2340</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B135" s="1" t="s">
         <v>191</v>
       </c>
@@ -8252,21 +8349,21 @@
         <v>20.147400000000001</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E136" s="2"/>
       <c r="F136" s="1" t="s">
         <v>164</v>
       </c>
       <c r="G136" s="2"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E137" s="2"/>
       <c r="G137" s="2"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E138" s="2"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" s="48">
         <v>14</v>
       </c>
@@ -8287,7 +8384,7 @@
         <v>31.62756278070735</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B140" s="1" t="s">
         <v>116</v>
       </c>
@@ -8309,7 +8406,7 @@
         <v>0.76964411329477977</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B141" s="1" t="s">
         <v>118</v>
       </c>
@@ -8331,7 +8428,7 @@
         <v>1.1309417716501837</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E142" s="2" t="s">
         <v>155</v>
       </c>
@@ -8344,7 +8441,7 @@
         <v>1.9005858849449635</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B143" s="1" t="s">
         <v>156</v>
       </c>
@@ -8354,13 +8451,13 @@
       </c>
       <c r="E143" s="2"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E144" s="2"/>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E145" s="2"/>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" s="48">
         <v>15</v>
       </c>
@@ -8368,12 +8465,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B147" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B148" s="1" t="s">
         <v>119</v>
       </c>
@@ -8385,7 +8482,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="151" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A151" s="49"/>
       <c r="B151" s="23" t="s">
         <v>202</v>
@@ -8397,7 +8494,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155" s="48">
         <v>16</v>
       </c>
@@ -8405,7 +8502,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B156" s="1" t="s">
         <v>95</v>
       </c>
@@ -8416,7 +8513,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B157" s="1" t="s">
         <v>96</v>
       </c>
@@ -8427,7 +8524,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B158" s="1" t="s">
         <v>97</v>
       </c>
@@ -8439,7 +8536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B159" s="1" t="s">
         <v>98</v>
       </c>
@@ -8454,7 +8551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B160" s="17" t="s">
         <v>152</v>
       </c>
@@ -8469,7 +8566,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="161" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="161" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B161" s="17" t="s">
         <v>153</v>
       </c>
@@ -8488,17 +8585,17 @@
         <v>87.858468162967654</v>
       </c>
     </row>
-    <row r="162" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="162" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B162" s="17"/>
       <c r="C162" s="7"/>
       <c r="E162" s="2"/>
     </row>
-    <row r="164" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="164" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B164" s="12" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="165" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="165" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B165" s="1" t="s">
         <v>46</v>
       </c>
@@ -8509,7 +8606,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="166" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="166" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B166" s="1" t="s">
         <v>50</v>
       </c>
@@ -8520,7 +8617,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="167" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="167" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B167" s="1" t="s">
         <v>51</v>
       </c>
@@ -8532,7 +8629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="168" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B168" s="1" t="s">
         <v>66</v>
       </c>
@@ -8547,7 +8644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="169" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B169" s="17" t="s">
         <v>107</v>
       </c>
@@ -8562,7 +8659,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="170" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="170" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B170" s="17" t="s">
         <v>108</v>
       </c>
@@ -8577,17 +8674,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="171" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="171" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B171" s="17"/>
       <c r="C171" s="7"/>
       <c r="E171" s="2"/>
     </row>
-    <row r="173" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="173" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B173" s="12" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="174" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="174" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B174" s="1" t="s">
         <v>129</v>
       </c>
@@ -8598,7 +8695,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="175" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="175" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B175" s="1" t="s">
         <v>130</v>
       </c>
@@ -8609,7 +8706,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="176" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="176" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B176" s="1" t="s">
         <v>128</v>
       </c>
@@ -8621,7 +8718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="177" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B177" s="1" t="s">
         <v>131</v>
       </c>
@@ -8636,7 +8733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="178" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B178" s="17" t="s">
         <v>141</v>
       </c>
@@ -8651,7 +8748,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="179" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="179" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B179" s="17" t="s">
         <v>142</v>
       </c>
@@ -8666,17 +8763,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="180" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="180" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B180" s="17"/>
       <c r="C180" s="7"/>
       <c r="E180" s="2"/>
     </row>
-    <row r="182" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="182" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B182" s="12" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="183" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="183" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B183" s="1" t="s">
         <v>133</v>
       </c>
@@ -8687,7 +8784,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="184" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="184" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B184" s="1" t="s">
         <v>134</v>
       </c>
@@ -8698,7 +8795,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="185" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="185" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B185" s="1" t="s">
         <v>135</v>
       </c>
@@ -8710,7 +8807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="186" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B186" s="1" t="s">
         <v>136</v>
       </c>
@@ -8725,7 +8822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="187" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B187" s="17" t="s">
         <v>138</v>
       </c>
@@ -8740,7 +8837,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="188" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="188" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B188" s="17" t="s">
         <v>140</v>
       </c>
@@ -8755,17 +8852,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="189" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="189" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B189" s="17"/>
       <c r="C189" s="7"/>
       <c r="E189" s="2"/>
     </row>
-    <row r="191" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="191" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B191" s="12" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="192" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="192" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B192" s="1" t="s">
         <v>173</v>
       </c>
@@ -8776,7 +8873,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="193" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="193" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B193" s="1" t="s">
         <v>144</v>
       </c>
@@ -8787,7 +8884,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="194" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="194" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B194" s="1" t="s">
         <v>145</v>
       </c>
@@ -8799,7 +8896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="195" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B195" s="1" t="s">
         <v>146</v>
       </c>
@@ -8814,7 +8911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="196" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B196" s="17" t="s">
         <v>147</v>
       </c>
@@ -8829,7 +8926,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="197" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="197" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B197" s="17" t="s">
         <v>148</v>
       </c>
@@ -8844,18 +8941,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="198" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="198" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B198" s="17"/>
       <c r="C198" s="7"/>
       <c r="E198" s="2"/>
     </row>
-    <row r="204" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="204" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B204" s="12"/>
     </row>
-    <row r="205" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="205" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E205" s="2"/>
     </row>
-    <row r="206" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="206" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E206" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Polished the equations and started work on the Submarine class
</commit_message>
<xml_diff>
--- a/Submarine/PodmornicaLast.xlsx
+++ b/Submarine/PodmornicaLast.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\STEM\git\Submarine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098B4D5F-582F-4819-8775-A96947798CA8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B068B081-ACDE-40C0-BB78-FEF660336B33}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3945" yWindow="1155" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Podmornica" sheetId="1" r:id="rId1"/>
@@ -23,13 +23,13 @@
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Podmornica!$I$92</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Podmornica!$D$84</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Podmornica!$D$88</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Podmornica!$D$84</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Podmornica!$D$86</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Podmornica!$D$87</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">Podmornica!$J$92</definedName>
-    <definedName name="solver_lhs5" localSheetId="0" hidden="1">Podmornica!$D$86</definedName>
+    <definedName name="solver_lhs5" localSheetId="0" hidden="1">Podmornica!$D$88</definedName>
     <definedName name="solver_lhs6" localSheetId="0" hidden="1">Podmornica!$D$85</definedName>
-    <definedName name="solver_lhs7" localSheetId="0" hidden="1">Podmornica!$D$87</definedName>
+    <definedName name="solver_lhs7" localSheetId="0" hidden="1">Podmornica!$I$92</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
@@ -41,20 +41,20 @@
     <definedName name="solver_opt" localSheetId="0" hidden="1">Podmornica!$H$98</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel5" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel6" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel7" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">Podmornica!$I$93</definedName>
+    <definedName name="solver_rel7" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">Podmornica!$J$94</definedName>
     <definedName name="solver_rhs5" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_rhs6" localSheetId="0" hidden="1">100</definedName>
-    <definedName name="solver_rhs7" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_rhs7" localSheetId="0" hidden="1">Podmornica!$I$93</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
@@ -2895,10 +2895,10 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>7.0250000000000004</c:v>
+                  <c:v>8.9699999999999989</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.0200456960690003</c:v>
+                  <c:v>8.9631180565175974</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2913,7 +2913,7 @@
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9161682770939992</c:v>
+                  <c:v>1.8057340387846461</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5852,8 +5852,8 @@
   </sheetPr>
   <dimension ref="A2:AQ206"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" colorId="8" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A19" colorId="8" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="H98" sqref="H98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -5942,7 +5942,7 @@
         <v>210</v>
       </c>
       <c r="D9" s="25">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -5950,7 +5950,7 @@
         <v>123</v>
       </c>
       <c r="D10" s="15">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>122</v>
@@ -5983,7 +5983,7 @@
         <v>209</v>
       </c>
       <c r="D13" s="25">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>27</v>
@@ -6048,11 +6048,11 @@
         <v>40</v>
       </c>
       <c r="D21" s="19">
-        <v>11.05</v>
+        <v>14.94</v>
       </c>
       <c r="F21" s="20">
         <f>E124</f>
-        <v>11.047767954145339</v>
+        <v>14.939594691926896</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -6092,7 +6092,7 @@
       </c>
       <c r="D25" s="1">
         <f>D21+2*D22</f>
-        <v>14.05</v>
+        <v>17.939999999999998</v>
       </c>
       <c r="I25" s="5"/>
     </row>
@@ -6102,7 +6102,7 @@
       </c>
       <c r="D26" s="5">
         <f>D36/(D25*2*D22*2*D22)</f>
-        <v>0.72949793824460485</v>
+        <v>0.74161900155812566</v>
       </c>
       <c r="I26" s="5"/>
     </row>
@@ -6124,7 +6124,7 @@
       </c>
       <c r="D29" s="2">
         <f>2*D22*PI()*D21</f>
-        <v>104.14379646650166</v>
+        <v>140.80618273389453</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>12</v>
@@ -6150,7 +6150,7 @@
       </c>
       <c r="D31" s="2">
         <f>D29+D30</f>
-        <v>132.4181303488098</v>
+        <v>169.08051661620266</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>12</v>
@@ -6175,7 +6175,7 @@
       </c>
       <c r="D34" s="2">
         <f>D22^2*PI()*D21</f>
-        <v>78.107847349876238</v>
+        <v>105.60463705042089</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>14</v>
@@ -6201,7 +6201,7 @@
       </c>
       <c r="D36" s="20">
         <f>D34+D35</f>
-        <v>92.245014291030301</v>
+        <v>119.74180399157495</v>
       </c>
       <c r="E36" s="16" t="s">
         <v>14</v>
@@ -6214,7 +6214,7 @@
       </c>
       <c r="D37" s="2">
         <f>D36*D3/1000</f>
-        <v>94.551139648306048</v>
+        <v>122.73534909136433</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>33</v>
@@ -6475,7 +6475,7 @@
       </c>
       <c r="F46" s="2">
         <f>D31*F39/1000*D4/1000*1.5</f>
-        <v>9.3881491303578208</v>
+        <v>11.987430277481801</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>33</v>
@@ -6495,7 +6495,7 @@
       </c>
       <c r="E50" s="47">
         <f>D13</f>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>27</v>
@@ -6514,7 +6514,7 @@
       </c>
       <c r="E51" s="3">
         <f>E50*H50</f>
-        <v>3.6011111111111114</v>
+        <v>6.1733333333333338</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>28</v>
@@ -6526,7 +6526,7 @@
       </c>
       <c r="E52" s="3">
         <f>E51/SQRT(9.08665*D25)</f>
-        <v>0.31871056437307255</v>
+        <v>0.48351127758467982</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
@@ -6535,7 +6535,7 @@
       </c>
       <c r="E53" s="9">
         <f>0.075/(LOG10(E54)-2)^2</f>
-        <v>2.3664460170731748E-3</v>
+        <v>2.1044004928933401E-3</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.3">
@@ -6544,7 +6544,7 @@
       </c>
       <c r="E54" s="9">
         <f>E51*(D25)/E55</f>
-        <v>42624777.684171118</v>
+        <v>93302106.14995788</v>
       </c>
       <c r="G54" s="8"/>
       <c r="H54" s="5"/>
@@ -6568,7 +6568,7 @@
       </c>
       <c r="E56" s="9">
         <f>E53*(1+E58)</f>
-        <v>4.1565197274068093E-3</v>
+        <v>3.0217233842543003E-3</v>
       </c>
       <c r="G56" s="8"/>
       <c r="H56" s="5"/>
@@ -6587,7 +6587,7 @@
       </c>
       <c r="E58" s="3">
         <f>-0.095+25.6*D26/(D25/(2*D22))^2</f>
-        <v>0.75643969793471189</v>
+        <v>0.43590699320723547</v>
       </c>
       <c r="H58" s="5"/>
     </row>
@@ -6597,7 +6597,7 @@
       </c>
       <c r="E59" s="2">
         <f>E56*0.5*D3*E51^2*D31/1000</f>
-        <v>3.6580042913755473</v>
+        <v>9.978875323711053</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>32</v>
@@ -6610,7 +6610,7 @@
       </c>
       <c r="E60" s="2">
         <f>E59*E51</f>
-        <v>13.172879898164611</v>
+        <v>61.602923665042908</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>31</v>
@@ -6623,7 +6623,7 @@
       </c>
       <c r="E61" s="2">
         <f>E60/(0.5*0.98)</f>
-        <v>26.883428363601247</v>
+        <v>125.72025237763859</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>31</v>
@@ -6635,7 +6635,7 @@
       </c>
       <c r="E62" s="13">
         <f>E61/E63</f>
-        <v>31.62756278070735</v>
+        <v>147.9061792678101</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>31</v>
@@ -6657,7 +6657,7 @@
       </c>
       <c r="E64" s="2">
         <f>E62*E148</f>
-        <v>3.1627562780707352</v>
+        <v>14.79061792678101</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>33</v>
@@ -6695,7 +6695,7 @@
       </c>
       <c r="F68" s="2">
         <f>C68*C135*E62</f>
-        <v>1.2651025112282941</v>
+        <v>5.9162471707124045</v>
       </c>
     </row>
     <row r="69" spans="1:32" x14ac:dyDescent="0.3">
@@ -6710,7 +6710,7 @@
       </c>
       <c r="E69" s="2">
         <f>C69*C135*E62/1000</f>
-        <v>1.1069646973247573</v>
+        <v>5.1767162743733532</v>
       </c>
     </row>
     <row r="71" spans="1:32" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -6793,7 +6793,7 @@
       <c r="H74" s="32"/>
       <c r="I74" s="33">
         <f>F46</f>
-        <v>9.3881491303578208</v>
+        <v>11.987430277481801</v>
       </c>
       <c r="J74" s="32">
         <f>D22+D24</f>
@@ -6804,16 +6804,16 @@
       </c>
       <c r="L74" s="34">
         <f>D25/2</f>
-        <v>7.0250000000000004</v>
+        <v>8.9699999999999989</v>
       </c>
       <c r="M74" s="32"/>
       <c r="N74" s="33">
         <f>I74*J74</f>
-        <v>20.653928086787207</v>
+        <v>26.372346610459964</v>
       </c>
       <c r="O74" s="33">
         <f>I74*L74</f>
-        <v>65.951747640763699</v>
+        <v>107.52724958901175</v>
       </c>
       <c r="P74" s="35"/>
       <c r="R74" s="2"/>
@@ -6850,7 +6850,7 @@
       <c r="K75" s="32"/>
       <c r="L75" s="34">
         <f>E195</f>
-        <v>12.047767954145339</v>
+        <v>15.939594691926898</v>
       </c>
       <c r="M75" s="32"/>
       <c r="N75" s="33">
@@ -6859,7 +6859,7 @@
       </c>
       <c r="O75" s="33">
         <f t="shared" ref="O75:O88" si="1">I75*L75</f>
-        <v>9.3972590042333657</v>
+        <v>12.432883859702981</v>
       </c>
       <c r="P75" s="35"/>
       <c r="R75" s="2"/>
@@ -6895,7 +6895,7 @@
       <c r="K76" s="32"/>
       <c r="L76" s="34">
         <f>E186</f>
-        <v>9.4583229274547467</v>
+        <v>12.455676407909269</v>
       </c>
       <c r="M76" s="32"/>
       <c r="N76" s="33">
@@ -6904,7 +6904,7 @@
       </c>
       <c r="O76" s="33">
         <f t="shared" si="1"/>
-        <v>9.4583229274547467</v>
+        <v>12.455676407909269</v>
       </c>
       <c r="P76" s="35"/>
       <c r="R76" s="2"/>
@@ -6932,7 +6932,7 @@
       <c r="H77" s="32"/>
       <c r="I77" s="33">
         <f>E64</f>
-        <v>3.1627562780707352</v>
+        <v>14.79061792678101</v>
       </c>
       <c r="J77" s="32">
         <f>D22+D24</f>
@@ -6941,16 +6941,16 @@
       <c r="K77" s="32"/>
       <c r="L77" s="34">
         <f>E177</f>
-        <v>7.2344389503820778</v>
+        <v>8.685879061945819</v>
       </c>
       <c r="M77" s="32"/>
       <c r="N77" s="33">
         <f t="shared" si="0"/>
-        <v>6.9580638117556184</v>
+        <v>32.539359438918225</v>
       </c>
       <c r="O77" s="33">
         <f t="shared" si="1"/>
-        <v>22.880767208640378</v>
+        <v>128.46951856346766</v>
       </c>
       <c r="P77" s="35"/>
       <c r="R77" s="2"/>
@@ -6978,7 +6978,7 @@
       <c r="H78" s="32"/>
       <c r="I78" s="33">
         <f>F142</f>
-        <v>1.8976537668424409</v>
+        <v>11.092963445085758</v>
       </c>
       <c r="J78" s="32">
         <f>D22/2+D24</f>
@@ -6987,16 +6987,16 @@
       <c r="K78" s="32"/>
       <c r="L78" s="34">
         <f>E177</f>
-        <v>7.2344389503820778</v>
+        <v>8.685879061945819</v>
       </c>
       <c r="M78" s="32"/>
       <c r="N78" s="33">
         <f t="shared" si="0"/>
-        <v>2.7515979619215396</v>
+        <v>16.084796995374351</v>
       </c>
       <c r="O78" s="33">
         <f t="shared" si="1"/>
-        <v>13.728460325184225</v>
+        <v>96.352138922600744</v>
       </c>
       <c r="P78" s="35"/>
       <c r="R78" s="2"/>
@@ -7034,7 +7034,7 @@
       </c>
       <c r="L79" s="34">
         <f>E168</f>
-        <v>6.35</v>
+        <v>7.15</v>
       </c>
       <c r="M79" s="32"/>
       <c r="N79" s="33">
@@ -7080,7 +7080,7 @@
       <c r="K80" s="32"/>
       <c r="L80" s="34">
         <f>E159</f>
-        <v>3.55</v>
+        <v>3.95</v>
       </c>
       <c r="M80" s="32"/>
       <c r="N80" s="33">
@@ -7089,7 +7089,7 @@
       </c>
       <c r="O80" s="33">
         <f t="shared" si="1"/>
-        <v>0.71</v>
+        <v>0.79</v>
       </c>
       <c r="P80" s="35"/>
       <c r="R80" s="2"/>
@@ -7126,7 +7126,7 @@
       <c r="K81" s="32"/>
       <c r="L81" s="34">
         <f>E159</f>
-        <v>3.55</v>
+        <v>3.95</v>
       </c>
       <c r="M81" s="32"/>
       <c r="N81" s="33">
@@ -7135,7 +7135,7 @@
       </c>
       <c r="O81" s="33">
         <f t="shared" si="1"/>
-        <v>1.42</v>
+        <v>1.58</v>
       </c>
       <c r="P81" s="35"/>
       <c r="R81" s="2"/>
@@ -7163,7 +7163,7 @@
       <c r="H82" s="32"/>
       <c r="I82" s="33">
         <f>E69</f>
-        <v>1.1069646973247573</v>
+        <v>5.1767162743733532</v>
       </c>
       <c r="J82" s="32">
         <f>D22/2+D24</f>
@@ -7172,7 +7172,7 @@
       <c r="K82" s="32"/>
       <c r="L82" s="34">
         <f>D25/2</f>
-        <v>7.0250000000000004</v>
+        <v>8.9699999999999989</v>
       </c>
       <c r="M82" s="32"/>
       <c r="N82" s="33"/>
@@ -7226,7 +7226,7 @@
       </c>
       <c r="C84" s="32"/>
       <c r="D84" s="33">
-        <v>53.040483349543663</v>
+        <v>54.431996323424634</v>
       </c>
       <c r="E84" s="33"/>
       <c r="F84" s="32"/>
@@ -7234,25 +7234,25 @@
       <c r="H84" s="32"/>
       <c r="I84" s="33">
         <f>E197*$D$3/1000*D84/100</f>
-        <v>4.4236522107547254</v>
+        <v>4.5397063839913532</v>
       </c>
       <c r="J84" s="34">
         <f>$D$23*D84/100</f>
-        <v>1.1668906336899607</v>
+        <v>1.197503919115342</v>
       </c>
       <c r="K84" s="37"/>
       <c r="L84" s="34">
         <f>E195</f>
-        <v>12.047767954145339</v>
+        <v>15.939594691926898</v>
       </c>
       <c r="M84" s="32"/>
       <c r="N84" s="33">
         <f t="shared" si="0"/>
-        <v>5.1619183314315773</v>
+        <v>5.4363161864625829</v>
       </c>
       <c r="O84" s="33">
         <f t="shared" si="1"/>
-        <v>53.295135345014963</v>
+        <v>72.361079781175221</v>
       </c>
       <c r="P84" s="35"/>
       <c r="R84" s="2"/>
@@ -7274,7 +7274,7 @@
       </c>
       <c r="C85" s="32"/>
       <c r="D85" s="33">
-        <v>99.038799351918129</v>
+        <v>100</v>
       </c>
       <c r="E85" s="33"/>
       <c r="F85" s="32"/>
@@ -7282,25 +7282,25 @@
       <c r="H85" s="32"/>
       <c r="I85" s="33">
         <f>E188*$D$3/1000*D85/100</f>
-        <v>34.517538182044412</v>
+        <v>49.772610957624671</v>
       </c>
       <c r="J85" s="34">
         <f t="shared" ref="J85:J88" si="2">$D$23*D85/100</f>
-        <v>2.1788535857421989</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="K85" s="37"/>
       <c r="L85" s="34">
         <f>E186</f>
-        <v>9.4583229274547467</v>
+        <v>12.455676407909269</v>
       </c>
       <c r="M85" s="32"/>
       <c r="N85" s="33">
         <f t="shared" si="0"/>
-        <v>75.208661838940728</v>
+        <v>109.49974410677429</v>
       </c>
       <c r="O85" s="33">
         <f t="shared" si="1"/>
-        <v>326.47802278652529</v>
+        <v>619.95153606493204</v>
       </c>
       <c r="P85" s="35"/>
       <c r="R85" s="2"/>
@@ -7322,7 +7322,7 @@
       </c>
       <c r="C86" s="32"/>
       <c r="D86" s="33">
-        <v>60.330817568385179</v>
+        <v>60.109571401344191</v>
       </c>
       <c r="E86" s="33"/>
       <c r="F86" s="32"/>
@@ -7330,25 +7330,25 @@
       <c r="H86" s="32"/>
       <c r="I86" s="33">
         <f>E179*$D$3/1000*D86/100</f>
-        <v>1.3529066191787538</v>
+        <v>7.8795759731628348</v>
       </c>
       <c r="J86" s="34">
         <f t="shared" si="2"/>
-        <v>1.3272779865044739</v>
+        <v>1.3224105708295724</v>
       </c>
       <c r="K86" s="37"/>
       <c r="L86" s="34">
         <f>E177</f>
-        <v>7.2344389503820778</v>
+        <v>8.685879061945819</v>
       </c>
       <c r="M86" s="32"/>
       <c r="N86" s="33">
         <f t="shared" si="0"/>
-        <v>1.7956831734321514</v>
+        <v>10.420034560565247</v>
       </c>
       <c r="O86" s="33">
         <f t="shared" si="1"/>
-        <v>9.7875203420165082</v>
+        <v>68.441043962306424</v>
       </c>
       <c r="P86" s="35"/>
       <c r="R86" s="2"/>
@@ -7370,7 +7370,7 @@
       </c>
       <c r="C87" s="32"/>
       <c r="D87" s="33">
-        <v>74.355331806265383</v>
+        <v>73.155519594023289</v>
       </c>
       <c r="E87" s="33"/>
       <c r="F87" s="32"/>
@@ -7378,27 +7378,27 @@
       <c r="H87" s="32"/>
       <c r="I87" s="33">
         <f>E170*$D$3/1000*D87/100</f>
-        <v>7.7516763412238241</v>
+        <v>7.6265937719767223</v>
       </c>
       <c r="J87" s="34">
         <f t="shared" si="2"/>
-        <v>1.6358172997378386</v>
+        <v>1.6094214310685127</v>
       </c>
       <c r="K87" s="37" t="s">
         <v>73</v>
       </c>
       <c r="L87" s="34">
         <f>E168</f>
-        <v>6.35</v>
+        <v>7.15</v>
       </c>
       <c r="M87" s="32"/>
       <c r="N87" s="33">
         <f t="shared" si="0"/>
-        <v>12.680326260942444</v>
+        <v>12.274403462672982</v>
       </c>
       <c r="O87" s="33">
         <f t="shared" si="1"/>
-        <v>49.223144766771277</v>
+        <v>54.530145469633567</v>
       </c>
       <c r="P87" s="35"/>
       <c r="R87" s="2"/>
@@ -7420,7 +7420,7 @@
       </c>
       <c r="C88" s="32"/>
       <c r="D88" s="33">
-        <v>83.550775667154738</v>
+        <v>69.276185239246345</v>
       </c>
       <c r="E88" s="33"/>
       <c r="F88" s="32"/>
@@ -7428,27 +7428,27 @@
       <c r="H88" s="32"/>
       <c r="I88" s="33">
         <f>E161*$D$3/1000*D88/100</f>
-        <v>28.569842422508582</v>
+        <v>28.310891607768973</v>
       </c>
       <c r="J88" s="34">
         <f t="shared" si="2"/>
-        <v>1.8381170646774043</v>
+        <v>1.5240760752634197</v>
       </c>
       <c r="K88" s="37" t="s">
         <v>72</v>
       </c>
       <c r="L88" s="34">
         <f>E159</f>
-        <v>3.55</v>
+        <v>3.95</v>
       </c>
       <c r="M88" s="32"/>
       <c r="N88" s="33">
         <f t="shared" si="0"/>
-        <v>52.51471489195746</v>
+        <v>43.147952568776624</v>
       </c>
       <c r="O88" s="33">
         <f t="shared" si="1"/>
-        <v>101.42294059990546</v>
+        <v>111.82802185068745</v>
       </c>
       <c r="P88" s="35"/>
       <c r="R88" s="2"/>
@@ -7555,25 +7555,25 @@
       <c r="H92" s="32"/>
       <c r="I92" s="39">
         <f>SUM(I73:I88)</f>
-        <v>94.551139648306048</v>
+        <v>143.55710661824648</v>
       </c>
       <c r="J92" s="40">
         <f>N92/I92</f>
-        <v>1.9161682770939992</v>
+        <v>1.8057340387846461</v>
       </c>
       <c r="K92" s="32"/>
       <c r="L92" s="41">
         <f>O92/I92</f>
-        <v>7.0200456960690003</v>
+        <v>8.9631180565175974</v>
       </c>
       <c r="M92" s="32"/>
       <c r="N92" s="33">
         <f>SUM(N73:N88)</f>
-        <v>181.17589435716872</v>
+        <v>259.22595393000427</v>
       </c>
       <c r="O92" s="33">
         <f>SUM(O73:O88)</f>
-        <v>663.75332094650992</v>
+        <v>1286.719294471427</v>
       </c>
       <c r="P92" s="35"/>
       <c r="R92" s="2"/>
@@ -7601,7 +7601,7 @@
       <c r="H93" s="32"/>
       <c r="I93" s="39">
         <f>D37</f>
-        <v>94.551139648306048</v>
+        <v>122.73534909136433</v>
       </c>
       <c r="J93" s="32"/>
       <c r="K93" s="32"/>
@@ -7660,7 +7660,7 @@
       <c r="K95" s="43"/>
       <c r="L95" s="44">
         <f>D25/2</f>
-        <v>7.0250000000000004</v>
+        <v>8.9699999999999989</v>
       </c>
       <c r="M95" s="43"/>
       <c r="N95" s="43"/>
@@ -7685,18 +7685,18 @@
       </c>
       <c r="H98" s="46">
         <f>ATAN((D25/2-L92)/(J94-J92))*180/PI()</f>
-        <v>1.0000005608104019</v>
+        <v>1.0000008034478562</v>
       </c>
       <c r="I98" s="47" t="s">
         <v>54</v>
       </c>
       <c r="M98" s="21">
         <f>D25/2</f>
-        <v>7.0250000000000004</v>
+        <v>8.9699999999999989</v>
       </c>
       <c r="N98" s="21">
         <f>L92</f>
-        <v>7.0200456960690003</v>
+        <v>8.9631180565175974</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.3">
@@ -7709,7 +7709,7 @@
       </c>
       <c r="N99" s="21">
         <f>J92</f>
-        <v>1.9161682770939992</v>
+        <v>1.8057340387846461</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.3">
@@ -7719,7 +7719,7 @@
       </c>
       <c r="N100" s="3">
         <f>M99-N99</f>
-        <v>0.283831722906001</v>
+        <v>0.39426596121535407</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.3">
@@ -7728,7 +7728,7 @@
       </c>
       <c r="N101" s="3">
         <f>N98-M98</f>
-        <v>-4.9543039310000481E-3</v>
+        <v>-6.8819434824014536E-3</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.3">
@@ -7745,7 +7745,7 @@
       </c>
       <c r="N103" s="2">
         <f>ATAN(N101/N100)*180/PI()</f>
-        <v>-1.0000005608104019</v>
+        <v>-1.0000008034478562</v>
       </c>
       <c r="O103" s="1" t="s">
         <v>54</v>
@@ -7775,7 +7775,7 @@
       </c>
       <c r="G106" s="5">
         <f>MAX(0,SIGN(2*D22-G104))*D21+2*SQRT(MAX(0, D22^2-(D22-G104)^2))</f>
-        <v>12.357669683062204</v>
+        <v>16.247669683062202</v>
       </c>
       <c r="H106" s="1" t="s">
         <v>0</v>
@@ -7799,7 +7799,7 @@
       </c>
       <c r="G108" s="3">
         <f>(D22^2*(PI()-ACOS(MIN(1, (G104-D22)/D22)))+(G104-D22)*G107/2)*D21</f>
-        <v>76.647774490131852</v>
+        <v>103.63056569073029</v>
       </c>
       <c r="H108" s="1" t="s">
         <v>14</v>
@@ -7823,7 +7823,7 @@
       </c>
       <c r="G110" s="3">
         <f>G108+G109</f>
-        <v>90.682446970962559</v>
+        <v>117.66523817156099</v>
       </c>
       <c r="H110" s="1" t="s">
         <v>14</v>
@@ -7835,7 +7835,7 @@
       </c>
       <c r="G111" s="3">
         <f>G112+G113-J92</f>
-        <v>1.8115960975978278</v>
+        <v>2.6469043329706388</v>
       </c>
       <c r="H111" s="1" t="s">
         <v>0</v>
@@ -7847,7 +7847,7 @@
       </c>
       <c r="G112" s="3">
         <f>G106*G107^3/12</f>
-        <v>2.3027643746918272</v>
+        <v>3.0276383717552844</v>
       </c>
       <c r="H112" s="1" t="s">
         <v>0</v>
@@ -7971,7 +7971,7 @@
       </c>
       <c r="E119" s="50">
         <f>2.5+D9*0.8</f>
-        <v>4.0999999999999996</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="F119" s="1" t="s">
         <v>0</v>
@@ -8050,7 +8050,7 @@
       </c>
       <c r="E121" s="18">
         <f>D143</f>
-        <v>0.26887790076415574</v>
+        <v>1.5717581238916385</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>0</v>
@@ -8068,7 +8068,7 @@
       </c>
       <c r="E122" s="18">
         <f>(15.385*E62+3692.3)/1000</f>
-        <v>4.178890053381183</v>
+        <v>5.9678365680352581</v>
       </c>
       <c r="F122" s="1" t="s">
         <v>0</v>
@@ -8129,7 +8129,7 @@
       <c r="D124" s="2"/>
       <c r="E124" s="2">
         <f>SUM(E119:E123)</f>
-        <v>11.047767954145339</v>
+        <v>14.939594691926896</v>
       </c>
       <c r="I124" s="1" t="s">
         <v>178</v>
@@ -8273,7 +8273,7 @@
       </c>
       <c r="C133" s="16">
         <f>D10</f>
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>122</v>
@@ -8381,7 +8381,7 @@
       </c>
       <c r="H139" s="2">
         <f>E62</f>
-        <v>31.62756278070735</v>
+        <v>147.9061792678101</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
@@ -8399,11 +8399,11 @@
       </c>
       <c r="F140" s="3">
         <f>C140*C133*$H$139/1000</f>
-        <v>0.60724920538958127</v>
+        <v>3.5497483024274423</v>
       </c>
       <c r="G140" s="3">
         <f>F140/(E140/1000)</f>
-        <v>0.76964411329477977</v>
+        <v>4.499047278108292</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.3">
@@ -8421,11 +8421,11 @@
       </c>
       <c r="F141" s="3">
         <f>C141*C133*$H$139/1000</f>
-        <v>1.2904045614528596</v>
+        <v>7.5432151426583154</v>
       </c>
       <c r="G141" s="3">
         <f>F141/(E141/1000)</f>
-        <v>1.1309417716501837</v>
+        <v>6.6110562161773139</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.3">
@@ -8434,11 +8434,11 @@
       </c>
       <c r="F142" s="3">
         <f>F140+F141</f>
-        <v>1.8976537668424409</v>
+        <v>11.092963445085758</v>
       </c>
       <c r="G142" s="3">
         <f>G140+G141</f>
-        <v>1.9005858849449635</v>
+        <v>11.110103494285607</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
@@ -8447,7 +8447,7 @@
       </c>
       <c r="D143" s="3">
         <f>G142/(D22^2*PI())</f>
-        <v>0.26887790076415574</v>
+        <v>1.5717581238916385</v>
       </c>
       <c r="E143" s="2"/>
     </row>
@@ -8545,7 +8545,7 @@
       </c>
       <c r="E159" s="3">
         <f>D22+E119/2</f>
-        <v>3.55</v>
+        <v>3.95</v>
       </c>
       <c r="F159" s="1" t="s">
         <v>0</v>
@@ -8560,7 +8560,7 @@
       </c>
       <c r="E160" s="2">
         <f>D22^2*PI()*E119</f>
-        <v>28.981192229365838</v>
+        <v>34.63605900582747</v>
       </c>
       <c r="F160" s="1" t="s">
         <v>14</v>
@@ -8575,14 +8575,14 @@
       </c>
       <c r="E161" s="2">
         <f>PI()*(360-E156-E157)/360*-(D22^2-E158^2)*E119</f>
-        <v>33.360572388470018</v>
+        <v>39.869952366708077</v>
       </c>
       <c r="F161" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G161" s="2">
         <f>E161+E170+E179+E188+E197</f>
-        <v>87.858468162967654</v>
+        <v>119.52519197007615</v>
       </c>
     </row>
     <row r="162" spans="2:7" x14ac:dyDescent="0.3">
@@ -8638,7 +8638,7 @@
       </c>
       <c r="E168" s="3">
         <f>D22+E119+E120/2</f>
-        <v>6.35</v>
+        <v>7.15</v>
       </c>
       <c r="F168" s="1" t="s">
         <v>0</v>
@@ -8727,7 +8727,7 @@
       </c>
       <c r="E177" s="3">
         <f>D22+E119+E120+E121/2</f>
-        <v>7.2344389503820778</v>
+        <v>8.685879061945819</v>
       </c>
       <c r="F177" s="1" t="s">
         <v>0</v>
@@ -8742,7 +8742,7 @@
       </c>
       <c r="E178" s="2">
         <f>D22^2*PI()*E121</f>
-        <v>1.9005858849449635</v>
+        <v>11.110103494285607</v>
       </c>
       <c r="F178" s="1" t="s">
         <v>14</v>
@@ -8757,7 +8757,7 @@
       </c>
       <c r="E179" s="2">
         <f>PI()*(360-E174-E175)/360*-(D22^2-E176^2)*E121</f>
-        <v>2.1877855297810918</v>
+        <v>12.788963577866546</v>
       </c>
       <c r="F179" s="1" t="s">
         <v>14</v>
@@ -8816,7 +8816,7 @@
       </c>
       <c r="E186" s="3">
         <f>D22+E119+E120+E121+E122/2</f>
-        <v>9.4583229274547467</v>
+        <v>12.455676407909269</v>
       </c>
       <c r="F186" s="1" t="s">
         <v>0</v>
@@ -8831,7 +8831,7 @@
       </c>
       <c r="E187" s="2">
         <f>D22^2*PI()*E122</f>
-        <v>29.538833156689012</v>
+        <v>42.184150919919205</v>
       </c>
       <c r="F187" s="1" t="s">
         <v>14</v>
@@ -8846,7 +8846,7 @@
       </c>
       <c r="E188" s="2">
         <f>PI()*(360-E183-E184)/360*-(D22^2-E185^2)*E122</f>
-        <v>34.002479055922024</v>
+        <v>48.558644836707003</v>
       </c>
       <c r="F188" s="1" t="s">
         <v>14</v>
@@ -8905,7 +8905,7 @@
       </c>
       <c r="E195" s="3">
         <f>D22+E119+E120+E121+E122+E123/2</f>
-        <v>12.047767954145339</v>
+        <v>15.939594691926898</v>
       </c>
       <c r="F195" s="1" t="s">
         <v>0</v>

</xml_diff>